<commit_message>
feat: incorporate my majority answer thing
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/categories.xlsx
+++ b/06-03-2023/data/output/xlsx/categories.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
-  <si>
-    <t>count</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>E. Final answer and equations same</t>
   </si>
@@ -70,25 +67,10 @@
     <t>Non-determinism issues as we do not know why it can't handle by itself</t>
   </si>
   <si>
-    <t>Non-determinism as we do not know how it could gotten the problem right</t>
-  </si>
-  <si>
-    <t>Can get the right equations, perhaps there is something about the equations from ground truth that mess it up</t>
-  </si>
-  <si>
-    <t>ChatGPT is lying on the equations it reports</t>
-  </si>
-  <si>
-    <t>Gets everything right</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>MAYBE</t>
   </si>
 </sst>
 </file>
@@ -589,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,37 +582,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2">
         <v>0</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -650,22 +632,22 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -685,22 +667,22 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -720,22 +702,22 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -755,372 +737,22 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>178</v>
+        <v>550</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
         <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>6</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>25</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>11</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>7</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="2">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>53</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="2">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>413</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: mistah adam tsukimoto crusher
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/categories.xlsx
+++ b/06-03-2023/data/output/xlsx/categories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>E. Final answer and equations same</t>
   </si>
@@ -67,10 +67,25 @@
     <t>Non-determinism issues as we do not know why it can't handle by itself</t>
   </si>
   <si>
+    <t>Non-determinism as we do not know how it could gotten the problem right</t>
+  </si>
+  <si>
+    <t>Can get the right equations, perhaps there is something about the equations from ground truth that mess it up</t>
+  </si>
+  <si>
+    <t>ChatGPT is lying on the equations it reports</t>
+  </si>
+  <si>
+    <t>Gets everything right</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>MAYBE</t>
   </si>
 </sst>
 </file>
@@ -571,7 +586,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -632,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -647,7 +662,7 @@
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -667,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -682,7 +697,7 @@
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -702,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -717,7 +732,7 @@
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -737,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>550</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -752,7 +767,392 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>82</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>119</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="2">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>507</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:baked a lovely little pie :heart:
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/categories.xlsx
+++ b/06-03-2023/data/output/xlsx/categories.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+  <si>
+    <t>E. Final answer and equations same</t>
+  </si>
   <si>
     <t>count</t>
-  </si>
-  <si>
-    <t>E. Final answer and equations same</t>
   </si>
   <si>
     <t>Equations</t>
@@ -241,54 +241,66 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>List!$A$10:$A$17</c:f>
+              <c:f>List!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>List!$F$10:$F$17</c:f>
+              <c:f>List!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>413</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,66 +399,292 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>List!$A$2:$A$9</c:f>
+              <c:f>List!$A$10:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>List!$F$2:$F$9</c:f>
+              <c:f>List!$G$10:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>118</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>178</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="10"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>When equations != text to final</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ChatGPT stats</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E7366B"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="29CC7A"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showPercent val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>List!$A$51:$A$52</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Wrong</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List!$B$51:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="10"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>When equations = text to final</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>ChatGPT stats</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E7366B"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="29CC7A"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showPercent val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>List!$H$51:$H$52</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Wrong</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List!$I$51:$I$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,6 +775,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -891,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
         <v>118</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -926,10 +1224,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>88</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>12</v>
@@ -961,10 +1259,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
         <v>37</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
@@ -996,10 +1294,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>178</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
@@ -1031,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
         <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -1066,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
         <v>6</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>12</v>
@@ -1101,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
         <v>32</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>12</v>
@@ -1136,10 +1434,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
         <v>18</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
@@ -1171,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
         <v>25</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -1206,10 +1504,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
         <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>12</v>
@@ -1241,10 +1539,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <v>11</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
@@ -1276,10 +1574,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
         <v>7</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -1296,7 +1594,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -1308,63 +1606,136 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>53</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
         <v>413</v>
       </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
         <v>21</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:9">
+      <c r="A50" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="H50" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>